<commit_message>
Precio con separador de miles
</commit_message>
<xml_diff>
--- a/bot/datos/Jefes 2017-2.xlsx
+++ b/bot/datos/Jefes 2017-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8592" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="450">
   <si>
     <t>Nombre</t>
   </si>
@@ -962,9 +962,6 @@
     <t>Paul Brenner</t>
   </si>
   <si>
-    <t>Alvaro Caeviedes</t>
-  </si>
-  <si>
     <t>Majo Castañeda</t>
   </si>
   <si>
@@ -1371,6 +1368,21 @@
   </si>
   <si>
     <t>Camino Otonal 1545</t>
+  </si>
+  <si>
+    <t>Alvaro Caviedes</t>
+  </si>
+  <si>
+    <t>Seba</t>
+  </si>
+  <si>
+    <t>Magdalena Astudillo</t>
+  </si>
+  <si>
+    <t>Tomas Ovalle</t>
+  </si>
+  <si>
+    <t>Sebastian Delorenzo</t>
   </si>
 </sst>
 </file>
@@ -1898,7 +1910,7 @@
   </sheetPr>
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J21" sqref="J21"/>
     </sheetView>
@@ -2111,10 +2123,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>108</v>
@@ -2126,7 +2138,7 @@
         <v>56977051605</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>235</v>
@@ -2169,7 +2181,7 @@
         <v>300</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>301</v>
@@ -2190,7 +2202,7 @@
         <v>56963033603</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>235</v>
@@ -2579,13 +2591,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>33</v>
@@ -2603,7 +2615,7 @@
         <v>56997267212</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>237</v>
@@ -4196,13 +4208,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>434</v>
-      </c>
       <c r="C73" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>30</v>
@@ -4220,7 +4232,7 @@
         <v>56975580528</v>
       </c>
       <c r="I73" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J73" s="11" t="s">
         <v>235</v>
@@ -4228,7 +4240,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>83</v>
@@ -4244,13 +4256,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>441</v>
-      </c>
       <c r="C75" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>33</v>
@@ -4268,7 +4280,7 @@
         <v>56997792386</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J75" s="11" t="s">
         <v>237</v>
@@ -4360,8 +4372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A96"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4954,8 +4966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9F498B-AB9E-409B-886F-760EBABE5D80}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4971,21 +4983,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>309</v>
+      <c r="A2" s="8" t="s">
+        <v>445</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -4998,27 +5010,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>213</v>
@@ -5026,88 +5038,88 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>374</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>410</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>381</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>207</v>
@@ -5115,7 +5127,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -5125,7 +5137,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -5133,36 +5145,36 @@
         <v>236</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>387</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -5172,7 +5184,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>185</v>
@@ -5180,15 +5192,15 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>77</v>
@@ -5196,10 +5208,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>50</v>
@@ -5215,36 +5227,36 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>62</v>
@@ -5262,7 +5274,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>44</v>
@@ -5270,26 +5282,26 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B46" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>378</v>
-      </c>
       <c r="D46" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -5299,12 +5311,12 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>55</v>
@@ -5312,15 +5324,15 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>97</v>
@@ -5328,7 +5340,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -5336,51 +5348,51 @@
         <v>308</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>21</v>
@@ -5388,123 +5400,120 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B66" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>395</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B68" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>392</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="D70" s="8" t="s">
         <v>400</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="str">
-        <f>Personas!A73&amp; " " &amp; Personas!B73</f>
-        <v>Magdalena Astudillo</v>
+      <c r="A72" s="9" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="9" t="str">
-        <f>Personas!A74&amp; " " &amp; Personas!B74</f>
-        <v>Tomas Ovalle</v>
+      <c r="A73" s="9" t="s">
+        <v>448</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="9" t="str">
-        <f>Personas!A75&amp; " " &amp; Personas!B75</f>
-        <v>Sebastian Delorenzo</v>
+      <c r="A74" s="9" t="s">
+        <v>449</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -5657,8 +5666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C3DA73-D96C-43A9-AE04-1BEC297F83DB}">
   <dimension ref="A1:B97"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5673,12 +5682,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>309</v>
+      <c r="A2" s="8" t="s">
+        <v>445</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>300</v>
@@ -5694,7 +5703,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>248</v>
@@ -5702,7 +5711,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>91</v>
@@ -5710,23 +5719,23 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>213</v>
@@ -5734,47 +5743,47 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>70</v>
@@ -5782,7 +5791,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>70</v>
@@ -5790,15 +5799,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>46</v>
@@ -5806,7 +5815,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>14</v>
@@ -5814,15 +5823,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>11</v>
@@ -5830,15 +5839,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>90</v>
@@ -5854,7 +5863,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>159</v>
@@ -5865,28 +5874,28 @@
         <v>236</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>276</v>
@@ -5894,10 +5903,10 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -5910,7 +5919,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>185</v>
@@ -5918,7 +5927,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>77</v>
@@ -5926,7 +5935,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>77</v>
@@ -5934,7 +5943,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>19</v>
@@ -5950,31 +5959,31 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>94</v>
@@ -5982,7 +5991,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>62</v>
@@ -6006,7 +6015,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>44</v>
@@ -6014,15 +6023,15 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>77</v>
@@ -6030,10 +6039,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -6046,39 +6055,39 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>219</v>
@@ -6094,7 +6103,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>75</v>
@@ -6102,7 +6111,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>221</v>
@@ -6110,15 +6119,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>64</v>
@@ -6126,15 +6135,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>211</v>
@@ -6142,7 +6151,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>21</v>
@@ -6150,15 +6159,15 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>16</v>
@@ -6166,15 +6175,15 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>193</v>
@@ -6182,39 +6191,39 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>266</v>
@@ -6222,36 +6231,42 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="str">
-        <f>Personas!A73&amp; " " &amp; Personas!B73</f>
-        <v>Magdalena Astudillo</v>
+      <c r="A72" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="str">
-        <f>Personas!A74&amp; " " &amp; Personas!B74</f>
-        <v>Tomas Ovalle</v>
+      <c r="A73" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="str">
-        <f>Personas!A75&amp; " " &amp; Personas!B75</f>
-        <v>Sebastian Delorenzo</v>
+      <c r="A74" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>